<commit_message>
scale data to dimensions of dam
</commit_message>
<xml_diff>
--- a/analysis/analysis.xlsx
+++ b/analysis/analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Documents/School/2022/Methods/PSMT/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{EFBE2705-63FF-DC46-996A-8769A988FC32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{853AE885-E0CF-A34C-BDF0-7EBABCD52FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5000" yWindow="1920" windowWidth="26220" windowHeight="17440"/>
+    <workbookView xWindow="4520" yWindow="1320" windowWidth="26220" windowHeight="17440"/>
   </bookViews>
   <sheets>
     <sheet name="points" sheetId="1" r:id="rId1"/>

</xml_diff>